<commit_message>
Rename translation columns to 'Target language' instead of using language code
</commit_message>
<xml_diff>
--- a/gemet/thesaurus/tests/files/only_en.xlsx
+++ b/gemet/thesaurus/tests/files/only_en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arielpontes/Projects/eaudeweb/gemet/gemet/thesaurus/tests/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1921D2-0E18-4648-A6D5-216404BB43F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15FD215B-0665-854A-929A-3FCB3D710A88}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16620" xr2:uid="{C2FA998E-ED6B-D344-9CA7-84375AD37A64}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="180">
   <si>
     <t>Term</t>
   </si>
@@ -102,9 +102,6 @@
     <t>brown finance</t>
   </si>
   <si>
-    <t>finances </t>
-  </si>
-  <si>
     <t>non-sustainable financing and investments which support the fossil fuel industry or carbon intensive activities</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t>CMU</t>
   </si>
   <si>
-    <t>waste reduction </t>
-  </si>
-  <si>
     <t>recycling, reuse, refurbishment and remanufacturing to reduce the generation of waste as well as the economy's dependence on extraction and imports of raw materials</t>
   </si>
   <si>
@@ -147,18 +141,12 @@
     <t>community science</t>
   </si>
   <si>
-    <t>science </t>
-  </si>
-  <si>
     <t>Climate Action Bonds</t>
   </si>
   <si>
     <t>CAB</t>
   </si>
   <si>
-    <t>financial instrument </t>
-  </si>
-  <si>
     <t>bonds whose issue is linked to projects with a positive impact on the environment, such as energy efficiency, the production of energy from renewable sources and sustainable land use</t>
   </si>
   <si>
@@ -171,9 +159,6 @@
     <t>climate benchmark</t>
   </si>
   <si>
-    <t>environmental investment </t>
-  </si>
-  <si>
     <t>investment benchmark that incorporates, next to financial investment objectives, specific objectives related to greenhouse gas emission reductions and the transition to a low-carbon economy through the selection and weighting of underlying benchmark constituents  </t>
   </si>
   <si>
@@ -186,9 +171,6 @@
     <t>Net zero emissions economy; net-zero greenhouse gas emissions economy; climate neutrality economy </t>
   </si>
   <si>
-    <t>economy </t>
-  </si>
-  <si>
     <t>human activities which  result in no net effect on the climate system by balancing residual emissions with emission (carbon dioxide) removal as well as accounting for regional or local biogeophysical effects of human activities that affect surface albedo or local climate</t>
   </si>
   <si>
@@ -198,9 +180,6 @@
     <t>carbon border tax</t>
   </si>
   <si>
-    <t>environmental tax </t>
-  </si>
-  <si>
     <t>levy on imported goods to counter carbon leakage, in order to avoid industries in countries with stricter rules being penalised</t>
   </si>
   <si>
@@ -213,9 +192,6 @@
     <t>consumer acceptance</t>
   </si>
   <si>
-    <t>consumer behaviour </t>
-  </si>
-  <si>
     <t>combination of the perceived variables visual attractiveness, perceived usefulness, perceived ease of use and perceived risk of a product or service</t>
   </si>
   <si>
@@ -243,9 +219,6 @@
     <t>Driving forces, Pressure, State, Impact, Response framework</t>
   </si>
   <si>
-    <t>environmental impact assessment </t>
-  </si>
-  <si>
     <t>framework for integrated assessments where social and economic developments exert pressure on the environment by changing the state of the environment and impacting  human health, ecosystems and materials</t>
   </si>
   <si>
@@ -256,9 +229,6 @@
   </si>
   <si>
     <t>environmental certification</t>
-  </si>
-  <si>
-    <t>certification </t>
   </si>
   <si>
     <r>
@@ -282,9 +252,6 @@
     <t>EU Green Bond label</t>
   </si>
   <si>
-    <t>environmental investment</t>
-  </si>
-  <si>
     <t>any type of listed or unlisted bond or capital market debt instrument issued by a European or international issuer that is aligned with the EU GBS</t>
   </si>
   <si>
@@ -309,9 +276,6 @@
     <t>eutrophication</t>
   </si>
   <si>
-    <t>pollution effect </t>
-  </si>
-  <si>
     <t>enrichment of water by nutrients, especially compounds of nitrogen and/or phosphorus, causing an accelerated growth of algae and higher forms of plant life that produce an undesirable disturbance to the balance of organisms present in the water and to the quality of the water concerned</t>
   </si>
   <si>
@@ -324,9 +288,6 @@
     <t>FF; Farm-to-table</t>
   </si>
   <si>
-    <t>sustainable consumption </t>
-  </si>
-  <si>
     <t>component of the EU strategy for sustainable food aiming to keep food safe, nutritious and of high quality by enhancing the environmental sustainability of the food system, involving all actors along the value chain</t>
   </si>
   <si>
@@ -339,9 +300,6 @@
     <t>floodplain</t>
   </si>
   <si>
-    <t>flood </t>
-  </si>
-  <si>
     <t>area next to a river bed which is more or less frequently covered with water in times of high water discharges from adjacent rivers</t>
   </si>
   <si>
@@ -354,9 +312,6 @@
     <t>glacier retreat </t>
   </si>
   <si>
-    <t>glacier </t>
-  </si>
-  <si>
     <t>uphill retraction of the lowest point of a glacier because ice melts or ablates more quickly than snowfall can accumulate and form new glacial ice</t>
   </si>
   <si>
@@ -369,9 +324,6 @@
     <t>green job</t>
   </si>
   <si>
-    <t>green economy </t>
-  </si>
-  <si>
     <t>activity producing goods and services to measure, prevent, limit, minimise or correct environmental damage to water, air and soil, as well as problems related to waste, noise and eco-systems, including technologies, products and services that reduce environmental risk, minimise pollution and resources  </t>
   </si>
   <si>
@@ -394,9 +346,6 @@
   </si>
   <si>
     <t>ecolabelled product</t>
-  </si>
-  <si>
-    <t>labelling </t>
   </si>
   <si>
     <t>sustainable product designed to minimise its environmental impact during the whole life-cycle, and even after it is of no use, to reduce waste and maximise resource efficiency</t>
@@ -488,9 +437,6 @@
     <t>hot spell; warm spell</t>
   </si>
   <si>
-    <t>weather condition </t>
-  </si>
-  <si>
     <t>period of abnormally hot weather</t>
   </si>
   <si>
@@ -500,9 +446,6 @@
     <t>low-carbon transition</t>
   </si>
   <si>
-    <t>carbon economy </t>
-  </si>
-  <si>
     <t>process or change  towards a low carbon economy and society, through concrete steps, policies and legislation aimed to deliver major reductions in greenhouse gas emission across all economic sectors and activities in a way that maximises economic opportunities, is socially fair and protects the most vulnerable</t>
   </si>
   <si>
@@ -510,9 +453,6 @@
   </si>
   <si>
     <t>material resource efficiency</t>
-  </si>
-  <si>
-    <t>efficiency criterion </t>
   </si>
   <si>
     <t>efficient, sustainable use of resources by minimising the impact on the environment,  creating more with less throughout the entire lifecycle, from material extraction, resource use and maintenance to material recovery</t>
@@ -553,9 +493,6 @@
     <t>NBS</t>
   </si>
   <si>
-    <t>flexible approach to environmental protection</t>
-  </si>
-  <si>
     <t>cost-effective approach that uses nature to deliver a range of critical services (wetlands for flood mitigation, carbon sequestration, improved air quality) that provides environmental, social and economic benefits, helping to build resilience by bringing more natural features and processes into the cities, landscapes and seascapes through locally adapted, resource-efficient and systemic interventions</t>
   </si>
   <si>
@@ -568,9 +505,6 @@
     <t>net zero CO2; net zero carbon dioxide; carbon neutrality</t>
   </si>
   <si>
-    <t>carbon balance </t>
-  </si>
-  <si>
     <t>globally balanced anthropogenic CO2 emissions through anthropogenic CO2 removals over a specified period</t>
   </si>
   <si>
@@ -578,9 +512,6 @@
   </si>
   <si>
     <t>noise map</t>
-  </si>
-  <si>
-    <t>noise monitoring </t>
   </si>
   <si>
     <t>visual presentation of the distribution of sound-pressure levels due to given noise sources across a geographic area and for a defined time period</t>
@@ -619,9 +550,6 @@
     <t>overconsumption</t>
   </si>
   <si>
-    <t>consumption behaviour </t>
-  </si>
-  <si>
     <t>excessive consumption or use of goods and services (energy, land, water or materials) that cause harm or detrimental effects to humans and/or the environment, namely by exceeding the carrying capacity and life supporting systems of the planet and its ecosystems</t>
   </si>
   <si>
@@ -634,9 +562,6 @@
     <t>QA</t>
   </si>
   <si>
-    <t>noise</t>
-  </si>
-  <si>
     <t>area with a pleasant soundscape and in which noise, i.e. unwanted sound, is absent or at least not dominant </t>
   </si>
   <si>
@@ -649,9 +574,6 @@
     <t>risk-based approach to change</t>
   </si>
   <si>
-    <t>risk management </t>
-  </si>
-  <si>
     <t>change based on the identification, evaluation and prioritisation of the risks involved, followed by the application of resources to minimise, monitor and control the probability/impact of events or to maximise the realisation of opportunities</t>
   </si>
   <si>
@@ -670,9 +592,6 @@
     <t>sustainability risk assessment</t>
   </si>
   <si>
-    <t>risk assessment </t>
-  </si>
-  <si>
     <t>identifying and analysing potential events that may negatively impact sustainability and evaluating that risk</t>
   </si>
   <si>
@@ -685,9 +604,6 @@
     <t>sustainability screening</t>
   </si>
   <si>
-    <t>principle of sustainability </t>
-  </si>
-  <si>
     <t>initial analysis of the potential positive or negative contribution of a proposal to sustainability </t>
   </si>
   <si>
@@ -697,9 +613,6 @@
     <t>sustainable banking</t>
   </si>
   <si>
-    <t>banking </t>
-  </si>
-  <si>
     <t>integration of environmental, social and governance criteria into traditional banking operational and business activities</t>
   </si>
   <si>
@@ -721,9 +634,6 @@
     <t>SBT; Systems-Based Thinking; system-based thinking </t>
   </si>
   <si>
-    <t>global model </t>
-  </si>
-  <si>
     <t>system viewed in a holistic manner by examining the linkages and interactions between the elements that comprise the whole of the system</t>
   </si>
   <si>
@@ -736,9 +646,6 @@
     <t>systemic change</t>
   </si>
   <si>
-    <t>behavioural change </t>
-  </si>
-  <si>
     <t>change required when efforts to change one aspect of a system fail to fix the problem and the whole system needs to be transformed, namely the fundamental qualities of the system itself, through innovation, experimentation, constant learning and adaptation</t>
   </si>
   <si>
@@ -748,9 +655,6 @@
     <t>Taxonomy Regulation</t>
   </si>
   <si>
-    <t>regulation </t>
-  </si>
-  <si>
     <t>framework to facilitate sustainable investment by establishing an EU-wide classification system to provide firms and investors with a common framework for identifying to what degree economic activities can be considered to be 'environmentally sustainable'</t>
   </si>
   <si>
@@ -770,9 +674,6 @@
   </si>
   <si>
     <t>water abstraction</t>
-  </si>
-  <si>
-    <t>water extraction </t>
   </si>
   <si>
     <t>removal or diversion of water from the water environment</t>
@@ -1259,7 +1160,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="A13:XFD13"/>
+      <selection activeCell="D6" sqref="D6:D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1389,18 +1290,16 @@
         <v>24</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="D6" s="8"/>
       <c r="E6" s="1"/>
       <c r="F6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="H6" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="84" x14ac:dyDescent="0.2">
@@ -1408,18 +1307,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="D7" s="8"/>
       <c r="E7" s="1"/>
       <c r="F7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>31</v>
       </c>
       <c r="H7" s="1"/>
     </row>
@@ -1428,23 +1325,21 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>34</v>
-      </c>
+      <c r="D8" s="8"/>
       <c r="E8" s="1"/>
       <c r="F8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="70" x14ac:dyDescent="0.2">
@@ -1452,20 +1347,18 @@
         <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>40</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D9" s="13"/>
       <c r="E9" s="14"/>
       <c r="F9" s="8" t="s">
-        <v>210</v>
+        <v>177</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>211</v>
+        <v>178</v>
       </c>
       <c r="H9" s="14"/>
     </row>
@@ -1474,23 +1367,21 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>43</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D10" s="8"/>
       <c r="E10" s="1"/>
       <c r="F10" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="154" x14ac:dyDescent="0.2">
@@ -1498,18 +1389,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="8" t="s">
-        <v>48</v>
-      </c>
+      <c r="D11" s="8"/>
       <c r="E11" s="1"/>
       <c r="F11" s="8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H11" s="1"/>
     </row>
@@ -1518,20 +1407,18 @@
         <v>11</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>53</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D12" s="13"/>
       <c r="E12" s="14"/>
       <c r="F12" s="13" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>212</v>
+        <v>179</v>
       </c>
       <c r="H12" s="14"/>
     </row>
@@ -1540,23 +1427,21 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>57</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="D13" s="8"/>
       <c r="E13" s="1"/>
       <c r="F13" s="8" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="102" x14ac:dyDescent="0.2">
@@ -1564,18 +1449,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="8" t="s">
-        <v>62</v>
-      </c>
+      <c r="D14" s="8"/>
       <c r="E14" s="1"/>
       <c r="F14" s="8" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="H14" s="1"/>
     </row>
@@ -1584,23 +1467,21 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>25</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="D15" s="9"/>
       <c r="E15" s="1"/>
       <c r="F15" s="8" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="112" x14ac:dyDescent="0.2">
@@ -1608,23 +1489,21 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>72</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D16" s="8"/>
       <c r="E16" s="1"/>
       <c r="F16" s="8" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="80" x14ac:dyDescent="0.2">
@@ -1632,18 +1511,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="8" t="s">
-        <v>77</v>
-      </c>
+      <c r="D17" s="8"/>
       <c r="E17" s="1"/>
       <c r="F17" s="4" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H17" s="1"/>
     </row>
@@ -1652,18 +1529,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="9" t="s">
-        <v>81</v>
-      </c>
+      <c r="D18" s="9"/>
       <c r="E18" s="1"/>
       <c r="F18" s="8" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="H18" s="1"/>
     </row>
@@ -1672,23 +1547,21 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>81</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="D19" s="9"/>
       <c r="E19" s="1"/>
       <c r="F19" s="8" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="112" x14ac:dyDescent="0.2">
@@ -1696,18 +1569,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="8" t="s">
-        <v>90</v>
-      </c>
+      <c r="D20" s="8"/>
       <c r="E20" s="1"/>
       <c r="F20" s="8" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="H20" s="1"/>
     </row>
@@ -1716,23 +1587,21 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>95</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="D21" s="8"/>
       <c r="E21" s="1"/>
       <c r="F21" s="8" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="84" x14ac:dyDescent="0.2">
@@ -1740,18 +1609,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="8" t="s">
-        <v>100</v>
-      </c>
+      <c r="D22" s="8"/>
       <c r="E22" s="1"/>
       <c r="F22" s="8" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="H22" s="1"/>
     </row>
@@ -1760,20 +1627,18 @@
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>105</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="D23" s="8"/>
       <c r="E23" s="1"/>
       <c r="F23" s="8" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="H23" s="1"/>
     </row>
@@ -1782,23 +1647,21 @@
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>110</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="D24" s="8"/>
       <c r="E24" s="1"/>
       <c r="F24" s="8" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="126" x14ac:dyDescent="0.2">
@@ -1806,18 +1669,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="9" t="s">
-        <v>25</v>
-      </c>
+      <c r="D25" s="9"/>
       <c r="E25" s="1"/>
       <c r="F25" s="8" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="H25" s="1"/>
     </row>
@@ -1826,23 +1687,21 @@
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>119</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="D26" s="8"/>
       <c r="E26" s="1"/>
       <c r="F26" s="8" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="192" x14ac:dyDescent="0.2">
@@ -1850,18 +1709,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="D27" s="8"/>
       <c r="E27" s="1"/>
       <c r="F27" s="8" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="H27" s="1"/>
     </row>
@@ -1870,20 +1727,18 @@
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>128</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="D28" s="8"/>
       <c r="E28" s="1"/>
       <c r="F28" s="8" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="H28" s="1"/>
     </row>
@@ -1892,18 +1747,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="8" t="s">
-        <v>132</v>
-      </c>
+      <c r="D29" s="8"/>
       <c r="E29" s="1"/>
       <c r="F29" s="8" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="H29" s="1"/>
     </row>
@@ -1912,21 +1765,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="8" t="s">
-        <v>136</v>
-      </c>
+      <c r="D30" s="8"/>
       <c r="E30" s="1"/>
       <c r="F30" s="8" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="154" x14ac:dyDescent="0.2">
@@ -1934,20 +1785,18 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>142</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="D31" s="8"/>
       <c r="E31" s="1"/>
       <c r="F31" s="8" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="H31" s="1"/>
     </row>
@@ -1956,20 +1805,18 @@
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>147</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="D32" s="8"/>
       <c r="E32" s="1"/>
       <c r="F32" s="8" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="H32" s="1"/>
     </row>
@@ -1978,21 +1825,19 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="C33" s="1"/>
-      <c r="D33" s="8" t="s">
-        <v>151</v>
-      </c>
+      <c r="D33" s="8"/>
       <c r="E33" s="1"/>
       <c r="F33" s="8" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="224" x14ac:dyDescent="0.2">
@@ -2000,18 +1845,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
       <c r="C34" s="1"/>
-      <c r="D34" s="8" t="s">
-        <v>156</v>
-      </c>
+      <c r="D34" s="8"/>
       <c r="E34" s="1"/>
       <c r="F34" s="8" t="s">
-        <v>157</v>
+        <v>133</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="H34" s="1"/>
     </row>
@@ -2020,20 +1863,18 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>161</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="D35" s="8"/>
       <c r="E35" s="1"/>
       <c r="F35" s="8" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="H35" s="1"/>
     </row>
@@ -2042,20 +1883,18 @@
         <v>35</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>166</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="D36" s="8"/>
       <c r="E36" s="1"/>
       <c r="F36" s="8" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>168</v>
+        <v>142</v>
       </c>
       <c r="H36" s="1"/>
     </row>
@@ -2064,18 +1903,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>169</v>
+        <v>143</v>
       </c>
       <c r="C37" s="1"/>
-      <c r="D37" s="8" t="s">
-        <v>43</v>
-      </c>
+      <c r="D37" s="8"/>
       <c r="E37" s="1"/>
       <c r="F37" s="8" t="s">
-        <v>170</v>
+        <v>144</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>171</v>
+        <v>145</v>
       </c>
       <c r="H37" s="1"/>
     </row>
@@ -2084,21 +1921,19 @@
         <v>37</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="C38" s="1"/>
-      <c r="D38" s="8" t="s">
-        <v>173</v>
-      </c>
+      <c r="D38" s="8"/>
       <c r="E38" s="1"/>
       <c r="F38" s="8" t="s">
-        <v>174</v>
+        <v>147</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>175</v>
+        <v>148</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>176</v>
+        <v>149</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="98" x14ac:dyDescent="0.2">
@@ -2106,18 +1941,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C39" s="1"/>
-      <c r="D39" s="8" t="s">
-        <v>178</v>
-      </c>
+      <c r="D39" s="8"/>
       <c r="E39" s="1"/>
       <c r="F39" s="8" t="s">
-        <v>179</v>
+        <v>151</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>180</v>
+        <v>152</v>
       </c>
       <c r="H39" s="1"/>
     </row>
@@ -2126,18 +1959,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>181</v>
+        <v>153</v>
       </c>
       <c r="C40" s="1"/>
-      <c r="D40" s="8" t="s">
-        <v>182</v>
-      </c>
+      <c r="D40" s="8"/>
       <c r="E40" s="1"/>
       <c r="F40" s="8" t="s">
-        <v>183</v>
+        <v>154</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>184</v>
+        <v>155</v>
       </c>
       <c r="H40" s="1"/>
     </row>
@@ -2146,18 +1977,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>185</v>
+        <v>156</v>
       </c>
       <c r="C41" s="1"/>
-      <c r="D41" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="D41" s="8"/>
       <c r="E41" s="1"/>
       <c r="F41" s="8" t="s">
-        <v>186</v>
+        <v>157</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>187</v>
+        <v>158</v>
       </c>
       <c r="H41" s="1"/>
     </row>
@@ -2166,23 +1995,21 @@
         <v>41</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>188</v>
+        <v>159</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>190</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="D42" s="8"/>
       <c r="E42" s="1"/>
       <c r="F42" s="8" t="s">
-        <v>191</v>
+        <v>161</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>192</v>
+        <v>162</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>193</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="112" x14ac:dyDescent="0.2">
@@ -2190,18 +2017,16 @@
         <v>42</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>194</v>
+        <v>164</v>
       </c>
       <c r="C43" s="1"/>
-      <c r="D43" s="8" t="s">
-        <v>195</v>
-      </c>
+      <c r="D43" s="8"/>
       <c r="E43" s="1"/>
       <c r="F43" s="8" t="s">
-        <v>196</v>
+        <v>165</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>197</v>
+        <v>166</v>
       </c>
       <c r="H43" s="1"/>
     </row>
@@ -2210,21 +2035,19 @@
         <v>43</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>198</v>
+        <v>167</v>
       </c>
       <c r="C44" s="1"/>
-      <c r="D44" s="8" t="s">
-        <v>199</v>
-      </c>
+      <c r="D44" s="8"/>
       <c r="E44" s="1"/>
       <c r="F44" s="8" t="s">
-        <v>200</v>
+        <v>168</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>201</v>
+        <v>169</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>202</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="140" x14ac:dyDescent="0.2">
@@ -2232,18 +2055,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>203</v>
+        <v>171</v>
       </c>
       <c r="C45" s="1"/>
-      <c r="D45" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="D45" s="8"/>
       <c r="E45" s="1"/>
       <c r="F45" s="8" t="s">
-        <v>204</v>
+        <v>172</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>205</v>
+        <v>173</v>
       </c>
       <c r="H45" s="1"/>
     </row>
@@ -2252,18 +2073,16 @@
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>206</v>
+        <v>174</v>
       </c>
       <c r="C46" s="1"/>
-      <c r="D46" s="8" t="s">
-        <v>207</v>
-      </c>
+      <c r="D46" s="8"/>
       <c r="E46" s="1"/>
       <c r="F46" s="8" t="s">
-        <v>208</v>
+        <v>175</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>209</v>
+        <v>176</v>
       </c>
       <c r="H46" s="1"/>
     </row>

</xml_diff>